<commit_message>
typo msic to misc
</commit_message>
<xml_diff>
--- a/data_excel/data_tables/excels/__tables__.xlsx
+++ b/data_excel/data_tables/excels/__tables__.xlsx
@@ -191,7 +191,7 @@
     <t>misc.tb_misc_param</t>
   </si>
   <si>
-    <t>msic_param</t>
+    <t>misc_param</t>
   </si>
   <si>
     <t>杂项参数表@Z-杂项表.xlsx</t>
@@ -1146,7 +1146,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>